<commit_message>
corrigindo B.I de Compras
</commit_message>
<xml_diff>
--- a/JellyFin_Server.xlsx
+++ b/JellyFin_Server.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Movies SELECTED" sheetId="1" state="visible" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="2953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="2954">
   <si>
     <t>Title</t>
   </si>
@@ -8891,6 +8891,9 @@
   </si>
   <si>
     <t xml:space="preserve">Radiofobia Classics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carioquismo Cultural</t>
   </si>
 </sst>
 </file>
@@ -37508,6 +37511,14 @@
         <v>2934</v>
       </c>
     </row>
+    <row r="25" ht="14.25">
+      <c r="A25" t="s">
+        <v>2953</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2929</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
save the new entrys
</commit_message>
<xml_diff>
--- a/JellyFin_Server.xlsx
+++ b/JellyFin_Server.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Movies SELECTED" sheetId="1" state="visible" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="2954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2974" uniqueCount="2974">
   <si>
     <t>Title</t>
   </si>
@@ -8287,286 +8287,346 @@
     <t xml:space="preserve">The Sky Crawlers</t>
   </si>
   <si>
+    <t xml:space="preserve">Jin-Roh - The Wolf Brigade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiroyuki Okiura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record of the Lodoss War</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krvavá pani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viktor Kubal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Angel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrick Bokanowski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vampire Hunter D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toyoo Ashida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vampire Hunter D: Bloodlust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoshiaki Kawajiri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lensman: Secret of The Lens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wicked City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neo Tokyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demon City Shinjuku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Wind Named Amnesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ninja Scroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highlander: The Search for Vengeance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fist of the North Star </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle in the Sky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hayao Miyazaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Neighbor Totoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiki's Delivery Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porco Rosso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whisper of the Heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princess Mononoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirited Away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Howl's Moving Castle</t>
+  </si>
+  <si>
+    <t>Ponyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Wind Rises</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Boy and the Heron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tales from Earthsea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gorō Miyazaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Up on Poppy Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grave of the Fireflies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isao Takahata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only Yesterday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pom Poko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Neighbors the Yamadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Tale of the Princess Kaguya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cat Returns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiroyuki Morita</t>
+  </si>
+  <si>
+    <t>Arrietty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiromasa Yonebayashi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When Marnie Was There</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Iron Giant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brad Bird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Thief and the Cobbler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Adventures of Prince Achmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lotte Reiniger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street of Crocodiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brothers Quay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Secret of NIMH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don Bluth</t>
+  </si>
+  <si>
+    <t>Anomalisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie Kaufman &amp; Duke Johnson</t>
+  </si>
+  <si>
+    <t>Shigurui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hirotsugu Hamazaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serialized Animations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murdoch Murdoch</t>
+  </si>
+  <si>
+    <t>magnet:?xt=urn:btih:22d219e0d87f0948471784ecdfcf60e54db7ed7a&amp;dn=Murdoch%20Murdoch&amp;tr=http%3A%2F%2Fshare.camoe.cn%3A8080%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.torrent.eu.org%3A451%2Fannounce&amp;tr=http%3A%2F%2Ft.nyaatracker.com%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.doko.moe%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fasnet.pw%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Fthetracker.org%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tfile.co%3A80%2Fannounce&amp;tr=http%3A%2F%2Fpt.lax.mx%3A80%2Fannounce&amp;tr=udp%3A%2F%2Fsantost12.xyz%3A6969%2Fannounce&amp;tr=https%3A%2F%2Ftracker.bt-hash.com%3A443%2Fannounce&amp;tr=udp%3A%2F%2Fbt.xxx-tracker.com%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.vanitycore.co%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fzephir.monocul.us%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fgrifon.info%3A80%2Fannounce&amp;tr=http%3A%2F%2Fretracker.spark-rostov.ru%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftr.kxmp.cf%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.city9x.com%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Fbt.aoeex.com%3A8000%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tfile.me%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.tiny-vps.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fretracker.telecom.by%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.electro-torrent.pl%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.tvunderground.org.ru%3A3218%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.halfchub.club%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fretracker.nts.su%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Fwambo.club%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.dutchtracking.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftc.animereactor.ru%3A8082%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.justseed.it%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.leechers-paradise.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.opentrackr.org%3A1337%2Fannounce&amp;tr=https%3A%2F%2Fopen.kickasstracker.com%3A443%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.coppersurfer.tk%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fopen.stealth.si%3A80%2Fannounce&amp;tr=http%3A%2F%2Fretracker.mgts.by%3A80%2Fannounce&amp;tr=http%3A%2F%2Fretracker.bashtel.ru%3A80%2Fannounce&amp;tr=udp%3A%2F%2Finferno.demonoid.pw%3A3418%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.cypherpunks.ru%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.calculate.ru%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.grepler.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.flashtorrents.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.yoshi210.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.tiny-vps.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.internetwarriors.net%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Fmgtracker.org%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.yoshi210.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tiny-vps.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.filetracker.pl%3A8089%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.ex.ua%3A80%2Fannounce&amp;tr=http%3A%2F%2Fmgtracker.org%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.aletorrenty.pl%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.filetracker.pl%3A8089%2Fannounce&amp;tr=http%3A%2F%2Ftracker.ex.ua%2Fannounce&amp;tr=http%3A%2F%2Fmgtracker.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fretracker.krs-ix.ru%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker2.indowebster.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fthetracker.org%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.bittor.pw%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.kicks-ass.net%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.aletorrenty.pl%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.aletorrenty.pl%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.bittorrent.am%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.kicks-ass.net%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.kicks-ass.net%2Fannounce&amp;tr=http%3A%2F%2Ftracker.baravik.org%3A6970%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.com%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.com%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker4.piratux.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.internetwarriors.net%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.skyts.net%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker2.wasabii.com.tw%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker2.itzmx.com%3A6961%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.nl%2Fannounce&amp;tr=udp%3A%2F%2Fbt.xxx-tracker.com%3A2710%2Fannounce&amp;tr=http%3A%2F%2Fwww.wareztorrent.com%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.eddie4.nl%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.grepler.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.mg64.net%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.coppersurfer.tk%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.ex.ua%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.opentrackr.org%3A1337%2Fannounce&amp;tr=http%3A%2F%2Ftracker.edoardocolombo.eu%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.kicks-ass.net%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.nl%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.mg64.net%3A6881%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.flashtorrents.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker1.wasabii.com.tw%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tfile.me%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.bittor.pw%3A1337%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tvunderground.org.ru%3A3218%2Fannounce&amp;tr=http%3A%2F%2Ftracker.grepler.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.bittor.pw%3A1337%2Fannounce&amp;tr=http%3A%2F%2Ftracker.flashtorrents.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fretracker.gorcomnet.ru%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969&amp;tr=udp%3A%2F%2Fpublic.popcorn-tracker.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.ilibr.org%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.kuroy.me%3A5944%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.mg64.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.cyberia.is%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.devil-torrents.pl%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker2.christianbro.pw%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fretracker.lanta-net.ru%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.internetwarriors.net%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Fulfbrueggemann.no-ip.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftorrentsmd.eu%3A8080%2Fannounce&amp;tr=udp%3A%2F%2Fpeerfect.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.swateam.org.uk%3A2710%2Fannounce&amp;tr=http%3A%2F%2Fns349743.ip-91-121-106.eu%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftorrentsmd.me%3A8080%2Fannounce&amp;tr=http%3A%2F%2Fagusiq-torrents.pl%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ffxtt.ru%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.vanitycore.co%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fexplodie.org%3A6969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spicy City</t>
+  </si>
+  <si>
+    <t>Hellsing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umanosuke Iida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ergo Proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shūkō Murase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend of the Galactic Heros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noboru Ishiguro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armored Troopers Voton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryōsuke Takahashi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cockpit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neon Genesis Evangelion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hideaki Anno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serial Experiments Lain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryūtarō Nakamura</t>
+  </si>
+  <si>
+    <t>Lazarus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shinichirō Watanabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samurai Champloo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cowboy Bebop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macross Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michiko &amp; Hatchin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sayo Yamamoto</t>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Masayuki Kojima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tetsurō Araki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paranoia Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satoshi Kon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Perfect Blue</t>
   </si>
   <si>
-    <t xml:space="preserve">Satoshi Kon</t>
-  </si>
-  <si>
     <t>Paprika</t>
   </si>
   <si>
-    <t xml:space="preserve">Jin-Roh - The Wolf Brigade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiroyuki Okiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Record of the Lodoss War</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krvavá pani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viktor Kubal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Angel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patrick Bokanowski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vampire Hunter D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toyoo Ashida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vampire Hunter D: Bloodlust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yoshiaki Kawajiri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lensman: Secret of The Lens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wicked City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neo Tokyo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demon City Shinjuku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Wind Named Amnesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ninja Scroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highlander: The Search for Vengeance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fist of the North Star </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Castle in the Sky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hayao Miyazaki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My Neighbor Totoro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiki's Delivery Service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porco Rosso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whisper of the Heart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Princess Mononoke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirited Away</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Howl's Moving Castle</t>
-  </si>
-  <si>
-    <t>Ponyo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Wind Rises</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Boy and the Heron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tales from Earthsea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gorō Miyazaki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From Up on Poppy Hill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grave of the Fireflies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isao Takahata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only Yesterday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pom Poko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My Neighbors the Yamadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Tale of the Princess Kaguya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cat Returns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiroyuki Morita</t>
-  </si>
-  <si>
-    <t>Arrietty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiromasa Yonebayashi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When Marnie Was There</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Iron Giant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brad Bird</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Thief and the Cobbler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richard Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Adventures of Prince Achmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lotte Reiniger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street of Crocodiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brothers Quay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Secret of NIMH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don Bluth</t>
-  </si>
-  <si>
-    <t>Anomalisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charlie Kaufman &amp; Duke Johnson</t>
-  </si>
-  <si>
-    <t>Shigurui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hirotsugu Hamazaki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serialized Animations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murdoch Murdoch</t>
-  </si>
-  <si>
-    <t>magnet:?xt=urn:btih:22d219e0d87f0948471784ecdfcf60e54db7ed7a&amp;dn=Murdoch%20Murdoch&amp;tr=http%3A%2F%2Fshare.camoe.cn%3A8080%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.torrent.eu.org%3A451%2Fannounce&amp;tr=http%3A%2F%2Ft.nyaatracker.com%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.doko.moe%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fasnet.pw%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Fthetracker.org%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tfile.co%3A80%2Fannounce&amp;tr=http%3A%2F%2Fpt.lax.mx%3A80%2Fannounce&amp;tr=udp%3A%2F%2Fsantost12.xyz%3A6969%2Fannounce&amp;tr=https%3A%2F%2Ftracker.bt-hash.com%3A443%2Fannounce&amp;tr=udp%3A%2F%2Fbt.xxx-tracker.com%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.vanitycore.co%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fzephir.monocul.us%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fgrifon.info%3A80%2Fannounce&amp;tr=http%3A%2F%2Fretracker.spark-rostov.ru%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftr.kxmp.cf%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.city9x.com%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Fbt.aoeex.com%3A8000%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tfile.me%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.tiny-vps.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fretracker.telecom.by%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.electro-torrent.pl%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.tvunderground.org.ru%3A3218%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.halfchub.club%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fretracker.nts.su%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Fwambo.club%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.dutchtracking.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftc.animereactor.ru%3A8082%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.justseed.it%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.leechers-paradise.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.opentrackr.org%3A1337%2Fannounce&amp;tr=https%3A%2F%2Fopen.kickasstracker.com%3A443%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.coppersurfer.tk%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fopen.stealth.si%3A80%2Fannounce&amp;tr=http%3A%2F%2Fretracker.mgts.by%3A80%2Fannounce&amp;tr=http%3A%2F%2Fretracker.bashtel.ru%3A80%2Fannounce&amp;tr=udp%3A%2F%2Finferno.demonoid.pw%3A3418%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.cypherpunks.ru%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.calculate.ru%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.grepler.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.flashtorrents.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.yoshi210.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.tiny-vps.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.internetwarriors.net%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Fmgtracker.org%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.yoshi210.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tiny-vps.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.filetracker.pl%3A8089%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.ex.ua%3A80%2Fannounce&amp;tr=http%3A%2F%2Fmgtracker.org%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.aletorrenty.pl%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.filetracker.pl%3A8089%2Fannounce&amp;tr=http%3A%2F%2Ftracker.ex.ua%2Fannounce&amp;tr=http%3A%2F%2Fmgtracker.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fretracker.krs-ix.ru%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker2.indowebster.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fthetracker.org%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.bittor.pw%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.kicks-ass.net%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.aletorrenty.pl%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.aletorrenty.pl%3A2710%2Fannounce&amp;tr=http%3A%2F%2Ftracker.bittorrent.am%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.kicks-ass.net%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.kicks-ass.net%2Fannounce&amp;tr=http%3A%2F%2Ftracker.baravik.org%3A6970%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.com%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.com%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker4.piratux.com%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.internetwarriors.net%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.skyts.net%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker2.wasabii.com.tw%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker2.itzmx.com%3A6961%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.nl%2Fannounce&amp;tr=udp%3A%2F%2Fbt.xxx-tracker.com%3A2710%2Fannounce&amp;tr=http%3A%2F%2Fwww.wareztorrent.com%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.eddie4.nl%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.grepler.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.mg64.net%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.coppersurfer.tk%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.ex.ua%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.opentrackr.org%3A1337%2Fannounce&amp;tr=http%3A%2F%2Ftracker.edoardocolombo.eu%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.kicks-ass.net%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.dutchtracking.nl%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftracker.mg64.net%3A6881%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.flashtorrents.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker1.wasabii.com.tw%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tfile.me%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.bittor.pw%3A1337%2Fannounce&amp;tr=http%3A%2F%2Ftracker.tvunderground.org.ru%3A3218%2Fannounce&amp;tr=http%3A%2F%2Ftracker.grepler.com%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.bittor.pw%3A1337%2Fannounce&amp;tr=http%3A%2F%2Ftracker.flashtorrents.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Fretracker.gorcomnet.ru%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.sktorrent.net%3A6969&amp;tr=udp%3A%2F%2Fpublic.popcorn-tracker.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.ilibr.org%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.kuroy.me%3A5944%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.mg64.net%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.cyberia.is%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftracker.devil-torrents.pl%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker2.christianbro.pw%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fretracker.lanta-net.ru%3A2710%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.internetwarriors.net%3A1337%2Fannounce&amp;tr=udp%3A%2F%2Fulfbrueggemann.no-ip.org%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ftorrentsmd.eu%3A8080%2Fannounce&amp;tr=udp%3A%2F%2Fpeerfect.org%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.swateam.org.uk%3A2710%2Fannounce&amp;tr=http%3A%2F%2Fns349743.ip-91-121-106.eu%3A80%2Fannounce&amp;tr=http%3A%2F%2Ftorrentsmd.me%3A8080%2Fannounce&amp;tr=http%3A%2F%2Fagusiq-torrents.pl%3A6969%2Fannounce&amp;tr=http%3A%2F%2Ffxtt.ru%3A80%2Fannounce&amp;tr=udp%3A%2F%2Ftracker.vanitycore.co%3A6969%2Fannounce&amp;tr=udp%3A%2F%2Fexplodie.org%3A6969</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paranoia Agent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spicy City</t>
-  </si>
-  <si>
-    <t>Hellsing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Umanosuke Iida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ergo Proxy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shūkō Murase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend of the Galactic Heros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noboru Ishiguro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armored Troopers Voton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ryōsuke Takahashi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cockpit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neon Genesis Evangelion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serial Experiments Lain</t>
-  </si>
-  <si>
-    <t>Lazarus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michiko &amp; Hatchin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samurai Champloo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cowboy Bebop</t>
-  </si>
-  <si>
-    <t>Monster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death Note</t>
+    <t>Memories</t>
   </si>
   <si>
     <t>Mononoke</t>
   </si>
   <si>
+    <t xml:space="preserve">Kenji Nakamura</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ayakashi: Japanese Classic Horror</t>
   </si>
   <si>
+    <t xml:space="preserve">Tetsuo Imazawa</t>
+  </si>
+  <si>
     <t>Animatrix</t>
   </si>
   <si>
+    <t xml:space="preserve">Lilly e Lana Wachowski</t>
+  </si>
+  <si>
     <t>Baccano!</t>
   </si>
   <si>
-    <t xml:space="preserve">Ad Astra: Scipio to Hannibal</t>
+    <t xml:space="preserve">Takahiro Omori</t>
   </si>
   <si>
     <t xml:space="preserve">Vinland Saga</t>
   </si>
   <si>
+    <t xml:space="preserve">Shūhei Yabuta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazuo Yamazaki</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Rose of Versailles</t>
   </si>
   <si>
+    <t xml:space="preserve">Tadao Nagahama</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Diary of Tortov Roddle</t>
   </si>
   <si>
+    <t xml:space="preserve">Kunio Katō</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iblard Jikan</t>
   </si>
   <si>
+    <t xml:space="preserve">Naohisa Inoue</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Girl From the Other Side: Siuil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yūtarō Kubo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun of the White Mare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcell Jankovics</t>
   </si>
   <si>
     <t>Author</t>
@@ -8900,7 +8960,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -8955,6 +9015,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10.500000"/>
+      <color indexed="64"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.000000"/>
       <name val="Calibri"/>
@@ -9002,7 +9067,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9055,20 +9120,37 @@
     <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
       <protection hidden="0" locked="1"/>
@@ -35059,9 +35141,7 @@
       <c r="E17" s="17"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="B18" s="13" t="s">
-        <v>2687</v>
-      </c>
+      <c r="B18" s="13"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
@@ -35097,7 +35177,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView showZeros="1" topLeftCell="A88" zoomScale="100" workbookViewId="0">
+    <sheetView showZeros="1" topLeftCell="A95" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -35582,7 +35662,7 @@
       <c r="A34" s="8" t="s">
         <v>2748</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="21" t="s">
         <v>2744</v>
       </c>
       <c r="C34" t="s">
@@ -35631,7 +35711,7 @@
         <v>2708</v>
       </c>
       <c r="D37" s="13">
-        <v>1997</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="38">
@@ -35645,7 +35725,7 @@
         <v>2708</v>
       </c>
       <c r="D38" s="13">
-        <v>2006</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="39">
@@ -35655,11 +35735,11 @@
       <c r="B39" t="s">
         <v>2755</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" t="s">
         <v>2708</v>
       </c>
       <c r="D39" s="13">
-        <v>1999</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="40">
@@ -35667,55 +35747,55 @@
         <v>2756</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>2755</v>
+        <v>2757</v>
       </c>
       <c r="C40" t="s">
         <v>2708</v>
       </c>
       <c r="D40" s="13">
-        <v>1990</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>2757</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="A41" s="8" t="s">
         <v>2758</v>
       </c>
-      <c r="C41" t="s">
+      <c r="B41" s="8" t="s">
+        <v>2759</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D41" s="13">
-        <v>1980</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="8" t="s">
-        <v>2759</v>
+        <v>2760</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>2760</v>
-      </c>
-      <c r="C42" t="s">
+        <v>2761</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D42" s="13">
-        <v>1982</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="8" t="s">
+        <v>2762</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>2761</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>2762</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D43" s="13">
-        <v>1985</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="44">
@@ -35723,119 +35803,119 @@
         <v>2763</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D44" s="13">
-        <v>2001</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="8" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D45" s="13">
-        <v>1984</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="8" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D46" s="13">
-        <v>1987</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D47" s="13">
-        <v>1987</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="8" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D48" s="13">
-        <v>1988</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="8" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D49" s="13">
-        <v>1990</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="8" t="s">
-        <v>2770</v>
+      <c r="A50" s="11" t="s">
+        <v>2769</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>2764</v>
+        <v>2759</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D50" s="13">
-        <v>1993</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="8" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>2771</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>2764</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D51" s="13">
-        <v>2007</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="8" t="s">
         <v>2772</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>2762</v>
+      <c r="B52" s="1" t="s">
+        <v>2771</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>2708</v>
@@ -35849,139 +35929,139 @@
         <v>2773</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D53" s="13">
-        <v>1986</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D54" s="13">
-        <v>1986</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="8" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D55" s="13">
-        <v>1989</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="8" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D56" s="13">
-        <v>1992</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="8" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D57" s="13">
-        <v>1995</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="8" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D58" s="13">
-        <v>1997</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="8" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D59" s="13">
-        <v>2001</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="8" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D60" s="13">
-        <v>2004</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="8" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D61" s="13">
-        <v>2008</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="8" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>2783</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>2774</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D62" s="13">
-        <v>2013</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="63">
@@ -35989,13 +36069,13 @@
         <v>2784</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>2774</v>
+        <v>2783</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D63" s="13">
-        <v>2023</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="64">
@@ -36009,7 +36089,7 @@
         <v>2708</v>
       </c>
       <c r="D64" s="13">
-        <v>2006</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="65">
@@ -36023,7 +36103,7 @@
         <v>2708</v>
       </c>
       <c r="D65" s="13">
-        <v>2011</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="66">
@@ -36031,55 +36111,55 @@
         <v>2788</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>2789</v>
+        <v>2786</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D66" s="13">
-        <v>1988</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="8" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>2789</v>
+        <v>2786</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D67" s="13">
-        <v>1991</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="8" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>2789</v>
+        <v>2786</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D68" s="13">
-        <v>1994</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="8" t="s">
+        <v>2791</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>2792</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>2789</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D69" s="13">
-        <v>1999</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="70">
@@ -36087,447 +36167,594 @@
         <v>2793</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>2789</v>
+        <v>2794</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D70" s="13">
-        <v>2013</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="8" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>2794</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>2795</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D71" s="13">
-        <v>2002</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="8" t="s">
+      <c r="A72" t="s">
         <v>2796</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="8" t="s">
         <v>2797</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="8" t="s">
         <v>2708</v>
       </c>
       <c r="D72" s="13">
-        <v>2010</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="8" t="s">
         <v>2798</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>2797</v>
-      </c>
-      <c r="C73" s="11" t="s">
+      <c r="B73" s="8" t="s">
+        <v>2799</v>
+      </c>
+      <c r="C73" t="s">
         <v>2708</v>
       </c>
       <c r="D73" s="13">
-        <v>2014</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s">
-        <v>2799</v>
-      </c>
-      <c r="B74" s="8" t="s">
+      <c r="A74" s="8" t="s">
         <v>2800</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="B74" s="19" t="s">
+        <v>2801</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D74" s="13">
-        <v>1999</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="8" t="s">
-        <v>2801</v>
+        <v>2802</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>2802</v>
-      </c>
-      <c r="C75" t="s">
+        <v>2803</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D75" s="13">
-        <v>1993</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="8" t="s">
-        <v>2803</v>
-      </c>
-      <c r="B76" s="19" t="s">
         <v>2804</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>2805</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D76" s="13">
-        <v>1926</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="8" t="s">
-        <v>2805</v>
+        <v>2806</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>2806</v>
+        <v>2807</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>2708</v>
       </c>
       <c r="D77" s="13">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="8" t="s">
-        <v>2807</v>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25">
+      <c r="A78" t="s">
+        <v>2808</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>2808</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>2708</v>
+        <v>2809</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>2810</v>
       </c>
       <c r="D78" s="13">
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="8" t="s">
-        <v>2809</v>
-      </c>
-      <c r="B79" s="8" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25">
+      <c r="A79" t="s">
+        <v>2811</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>2811</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>2810</v>
       </c>
-      <c r="C79" s="11" t="s">
-        <v>2708</v>
-      </c>
       <c r="D79" s="13">
-        <v>2015</v>
+        <v>2016</v>
+      </c>
+      <c r="E79" t="s">
+        <v>2812</v>
       </c>
     </row>
     <row r="80" ht="14.25">
-      <c r="A80" t="s">
-        <v>2811</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>2812</v>
-      </c>
-      <c r="C80" s="8" t="s">
+      <c r="A80" s="8" t="s">
         <v>2813</v>
       </c>
+      <c r="B80" s="11" t="s">
+        <v>2719</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>2810</v>
+      </c>
       <c r="D80" s="13">
-        <v>2007</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="81" ht="14.25">
       <c r="A81" t="s">
         <v>2814</v>
       </c>
-      <c r="B81" s="11" t="s">
-        <v>2814</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>2813</v>
+      <c r="B81" s="19" t="s">
+        <v>2815</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>2810</v>
       </c>
       <c r="D81" s="13">
-        <v>2016</v>
-      </c>
-      <c r="E81" t="s">
-        <v>2815</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="82" ht="14.25">
-      <c r="A82" t="s">
-        <v>2816</v>
+      <c r="A82" s="11" t="s">
+        <v>2769</v>
       </c>
       <c r="B82" t="s">
-        <v>2752</v>
-      </c>
-      <c r="C82" t="s">
-        <v>2813</v>
+        <v>2759</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>2810</v>
       </c>
       <c r="D82" s="13">
-        <v>2004</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="8" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>2817</v>
       </c>
-      <c r="B83" s="11" t="s">
-        <v>2719</v>
-      </c>
       <c r="C83" s="11" t="s">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="D83" s="13">
-        <v>1997</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="84" ht="14.25">
       <c r="A84" t="s">
         <v>2818</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="B84" s="22" t="s">
         <v>2819</v>
       </c>
-      <c r="C84" s="11" t="s">
-        <v>2813</v>
+      <c r="C84" s="8" t="s">
+        <v>2810</v>
       </c>
       <c r="D84" s="13">
-        <v>1997</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="85" ht="14.25">
-      <c r="A85" s="11" t="s">
-        <v>2772</v>
-      </c>
-      <c r="B85" t="s">
-        <v>2762</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>2813</v>
+      <c r="A85" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>2821</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>2810</v>
       </c>
       <c r="D85" s="13">
-        <v>1984</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="86" ht="14.25">
-      <c r="A86" s="8" t="s">
-        <v>2820</v>
+      <c r="A86" t="s">
+        <v>2822</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>2821</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>2813</v>
+        <v>2761</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>2810</v>
       </c>
       <c r="D86" s="13">
-        <v>2006</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" t="s">
-        <v>2822</v>
+        <v>2823</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>2823</v>
+        <v>2824</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>2813</v>
-      </c>
-      <c r="D87" s="13">
-        <v>1988</v>
+        <v>2810</v>
+      </c>
+      <c r="D87" s="20">
+        <v>1995</v>
       </c>
     </row>
     <row r="88" ht="14.25">
       <c r="A88" t="s">
-        <v>2824</v>
-      </c>
-      <c r="B88" s="8" t="s">
         <v>2825</v>
       </c>
+      <c r="B88" s="21" t="s">
+        <v>2826</v>
+      </c>
       <c r="C88" s="8" t="s">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="D88" s="13">
-        <v>1983</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="89" ht="14.25">
-      <c r="A89" t="s">
-        <v>2826</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>2764</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>2813</v>
+      <c r="A89" s="8" t="s">
+        <v>2827</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>2828</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2810</v>
       </c>
       <c r="D89" s="13">
-        <v>1993</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="90" ht="14.25">
       <c r="A90" t="s">
-        <v>2827</v>
+        <v>2829</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2828</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>2813</v>
-      </c>
-      <c r="D90" s="20">
-        <v>1995</v>
+        <v>2810</v>
+      </c>
+      <c r="D90" s="13">
+        <v>2004</v>
       </c>
     </row>
     <row r="91" ht="14.25">
       <c r="A91" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B91" t="s">
         <v>2828</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>2813</v>
-      </c>
-      <c r="D91" s="13">
+      <c r="C91" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D91" s="20">
         <v>1998</v>
       </c>
     </row>
     <row r="92" ht="14.25">
-      <c r="A92" s="8" t="s">
-        <v>2829</v>
-      </c>
-      <c r="C92"/>
-      <c r="D92" s="13"/>
+      <c r="A92" s="21" t="s">
+        <v>2831</v>
+      </c>
+      <c r="B92" s="23" t="s">
+        <v>2828</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D92" s="13">
+        <v>1994</v>
+      </c>
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="8" t="s">
-        <v>2830</v>
-      </c>
-      <c r="C93"/>
-      <c r="D93" s="13"/>
+        <v>2832</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>2833</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D93" s="13">
+        <v>2008</v>
+      </c>
     </row>
     <row r="94" ht="14.25">
       <c r="A94" t="s">
-        <v>2831</v>
+        <v>2834</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>2835</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="D94" s="13">
         <v>2004</v>
       </c>
     </row>
     <row r="95" ht="14.25">
-      <c r="A95" t="s">
-        <v>2832</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>2813</v>
-      </c>
-      <c r="D95" s="20">
-        <v>1998</v>
+      <c r="A95" s="8" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>2837</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D95" s="13">
+        <v>2006</v>
       </c>
     </row>
     <row r="96" ht="14.25">
       <c r="A96" t="s">
-        <v>2833</v>
+        <v>2838</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>2839</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="D96" s="13">
         <v>2004</v>
       </c>
     </row>
     <row r="97" ht="14.25">
-      <c r="A97" s="8" t="s">
-        <v>2834</v>
-      </c>
-      <c r="C97" t="s">
-        <v>2813</v>
+      <c r="A97" t="s">
+        <v>2840</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2839</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D97" s="13">
+        <v>1997</v>
       </c>
     </row>
     <row r="98" ht="14.25">
-      <c r="A98" t="s">
-        <v>2816</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>2813</v>
+      <c r="A98" s="8" t="s">
+        <v>2841</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>2839</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2708</v>
       </c>
       <c r="D98" s="13">
-        <v>2004</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="99" ht="14.25">
-      <c r="A99" s="22" t="s">
-        <v>2835</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>2813</v>
+      <c r="A99" s="21" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>2740</v>
+      </c>
+      <c r="C99" s="25" t="s">
+        <v>2708</v>
       </c>
       <c r="D99" s="13">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25">
+      <c r="A100" s="26" t="s">
+        <v>2843</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>2844</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D100" s="13">
         <v>2006</v>
       </c>
     </row>
-    <row r="100" ht="14.25">
-      <c r="A100" s="22" t="s">
-        <v>2836</v>
-      </c>
-      <c r="C100" t="s">
-        <v>2813</v>
-      </c>
-      <c r="D100" s="13"/>
-    </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="8" t="s">
-        <v>2837</v>
+      <c r="A101" s="26" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>2846</v>
       </c>
       <c r="C101" t="s">
-        <v>2813</v>
+        <v>2810</v>
+      </c>
+      <c r="D101" s="13">
+        <v>2006</v>
       </c>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="8" t="s">
-        <v>2838</v>
+        <v>2847</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>2848</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D102" s="13">
+        <v>2003</v>
       </c>
     </row>
     <row r="103" ht="14.25">
       <c r="A103" s="8" t="s">
-        <v>2839</v>
+        <v>2849</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>2850</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D103" s="13">
+        <v>2007</v>
       </c>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="8" t="s">
-        <v>2840</v>
+        <v>2851</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>2852</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D104" s="13">
+        <v>2019</v>
       </c>
     </row>
     <row r="105" ht="14.25">
-      <c r="A105" s="8"/>
+      <c r="A105" s="8" t="s">
+        <v>2766</v>
+      </c>
+      <c r="B105" s="27" t="s">
+        <v>2853</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D105" s="13">
+        <v>1990</v>
+      </c>
     </row>
     <row r="106" ht="14.25">
       <c r="A106" s="8" t="s">
-        <v>2769</v>
+        <v>2854</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>2855</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D106" s="13">
+        <v>1979</v>
       </c>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="8" t="s">
-        <v>2841</v>
+        <v>2790</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>2786</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D107" s="28">
+        <v>2013</v>
       </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="8" t="s">
-        <v>2793</v>
+        <v>2856</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>2857</v>
+      </c>
+      <c r="C108" s="21" t="s">
+        <v>2858</v>
+      </c>
+      <c r="D108" s="13">
+        <v>2003</v>
       </c>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="8" t="s">
-        <v>2842</v>
+        <v>2859</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>2860</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D109" s="13">
+        <v>2007</v>
       </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="8" t="s">
-        <v>2843</v>
+        <v>2861</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>2862</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D110" s="13">
+        <v>2019</v>
       </c>
     </row>
     <row r="111" ht="14.25">
-      <c r="A111" s="8" t="s">
-        <v>2844</v>
-      </c>
+      <c r="A111" s="21" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>2864</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D111" s="13">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="112" ht="14.25">
+      <c r="A112"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -36554,30 +36781,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>2845</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="29" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="24" t="s">
-        <v>2846</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="A2" s="30" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="17" t="s">
@@ -36586,665 +36815,665 @@
       <c r="B3" s="17" t="s">
         <v>2740</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="17" t="s">
-        <v>2848</v>
+        <v>2868</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>2849</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+        <v>2869</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="17" t="s">
-        <v>2850</v>
+        <v>2870</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>2851</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+        <v>2871</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="17" t="s">
-        <v>2852</v>
+        <v>2872</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>2853</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+        <v>2873</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="17" t="s">
-        <v>2854</v>
+        <v>2874</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="17" t="s">
-        <v>2855</v>
+        <v>2875</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>2856</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+        <v>2876</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="17" t="s">
-        <v>2857</v>
+        <v>2877</v>
       </c>
       <c r="B9" s="17"/>
-      <c r="C9" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="C9" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="17" t="s">
-        <v>2858</v>
+        <v>2878</v>
       </c>
       <c r="B10" s="17"/>
-      <c r="C10" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="17" t="s">
-        <v>2859</v>
+        <v>2879</v>
       </c>
       <c r="B11" s="17"/>
-      <c r="C11" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="17" t="s">
-        <v>2833</v>
+        <v>2834</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
+      <c r="C12" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="17" t="s">
-        <v>2860</v>
+        <v>2880</v>
       </c>
       <c r="B13" s="17"/>
-      <c r="C13" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="C13" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="17" t="s">
-        <v>2861</v>
+        <v>2881</v>
       </c>
       <c r="B14" s="17"/>
-      <c r="C14" s="26" t="s">
-        <v>2847</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="C14" s="33" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="17" t="s">
-        <v>2862</v>
+        <v>2882</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>2863</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>2864</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26" t="s">
-        <v>2865</v>
+        <v>2883</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>2884</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33" t="s">
+        <v>2885</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="17" t="s">
-        <v>2866</v>
+        <v>2886</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>2867</v>
+        <v>2887</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>2864</v>
+        <v>2884</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="17" t="s">
-        <v>2868</v>
+        <v>2888</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>2869</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>2864</v>
-      </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
+        <v>2889</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>2884</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="17" t="s">
-        <v>2870</v>
+        <v>2890</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>2871</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>2864</v>
-      </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
+        <v>2891</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>2884</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="17" t="s">
-        <v>2872</v>
+        <v>2892</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>2873</v>
+        <v>2893</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>2874</v>
-      </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26" t="s">
-        <v>2875</v>
+        <v>2894</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33" t="s">
+        <v>2895</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="17" t="s">
-        <v>2876</v>
+        <v>2896</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>2877</v>
+        <v>2897</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>2874</v>
-      </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+        <v>2894</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="17" t="s">
-        <v>2878</v>
+        <v>2898</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>2879</v>
+        <v>2899</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>2874</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26" t="s">
-        <v>2880</v>
+        <v>2894</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33" t="s">
+        <v>2900</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="17" t="s">
-        <v>2881</v>
+        <v>2901</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>2882</v>
+        <v>2902</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>2882</v>
+        <v>2902</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="17" t="s">
-        <v>2883</v>
+        <v>2903</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>2882</v>
+        <v>2902</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>2882</v>
+        <v>2902</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="17" t="s">
-        <v>2884</v>
+        <v>2904</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>2885</v>
+        <v>2905</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>2885</v>
-      </c>
-      <c r="D24" s="26"/>
+        <v>2905</v>
+      </c>
+      <c r="D24" s="33"/>
       <c r="E24" s="17"/>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="17" t="s">
-        <v>2886</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>2887</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>2888</v>
-      </c>
-      <c r="D25" s="26"/>
+        <v>2906</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>2907</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>2908</v>
+      </c>
+      <c r="D25" s="33"/>
       <c r="E25" s="17"/>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="17" t="s">
-        <v>2889</v>
+        <v>2909</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>2890</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D26" s="26"/>
+        <v>2910</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>2911</v>
+      </c>
+      <c r="D26" s="33"/>
       <c r="E26" s="17"/>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="17" t="s">
-        <v>2892</v>
+        <v>2912</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>2891</v>
+        <v>2911</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D27" s="26"/>
+        <v>2911</v>
+      </c>
+      <c r="D27" s="33"/>
       <c r="E27" s="17"/>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="17" t="s">
-        <v>2893</v>
+        <v>2913</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>2891</v>
+        <v>2911</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D28" s="26"/>
+        <v>2911</v>
+      </c>
+      <c r="D28" s="33"/>
       <c r="E28" s="17"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="17" t="s">
-        <v>2894</v>
+        <v>2914</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>2891</v>
+        <v>2911</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D29" s="26"/>
+        <v>2911</v>
+      </c>
+      <c r="D29" s="33"/>
       <c r="E29" s="17"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="17" t="s">
-        <v>2895</v>
+        <v>2915</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>2891</v>
+        <v>2911</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D30" s="26"/>
+        <v>2911</v>
+      </c>
+      <c r="D30" s="33"/>
       <c r="E30" s="17"/>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="17" t="s">
-        <v>2896</v>
+        <v>2916</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>2891</v>
+        <v>2911</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D31" s="26"/>
+        <v>2911</v>
+      </c>
+      <c r="D31" s="33"/>
       <c r="E31" s="17"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="17" t="s">
-        <v>2897</v>
+        <v>2917</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>2891</v>
+        <v>2911</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>2891</v>
-      </c>
-      <c r="D32" s="26"/>
+        <v>2911</v>
+      </c>
+      <c r="D32" s="33"/>
       <c r="E32" s="17"/>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="17" t="s">
-        <v>2898</v>
+        <v>2918</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>2899</v>
+        <v>2919</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D33" s="26"/>
+        <v>2919</v>
+      </c>
+      <c r="D33" s="33"/>
       <c r="E33" s="17"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="17" t="s">
-        <v>2900</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>2899</v>
+        <v>2920</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>2919</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D34" s="26"/>
+        <v>2919</v>
+      </c>
+      <c r="D34" s="33"/>
       <c r="E34" s="17"/>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="17" t="s">
-        <v>2901</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>2899</v>
+        <v>2921</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>2919</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D35" s="26"/>
+        <v>2919</v>
+      </c>
+      <c r="D35" s="33"/>
       <c r="E35" s="17"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="17" t="s">
-        <v>2902</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>2899</v>
+        <v>2922</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>2919</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D36" s="26"/>
+        <v>2919</v>
+      </c>
+      <c r="D36" s="33"/>
       <c r="E36" s="17"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="17" t="s">
-        <v>2903</v>
+        <v>2923</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>2417</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>2904</v>
-      </c>
-      <c r="D37" s="26"/>
+      <c r="C37" s="33" t="s">
+        <v>2924</v>
+      </c>
+      <c r="D37" s="33"/>
       <c r="E37" s="17"/>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="17" t="s">
-        <v>2905</v>
+        <v>2925</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>2417</v>
       </c>
-      <c r="C38" s="26" t="s">
-        <v>2904</v>
-      </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26" t="s">
-        <v>2906</v>
+      <c r="C38" s="33" t="s">
+        <v>2924</v>
+      </c>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33" t="s">
+        <v>2926</v>
       </c>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="17" t="s">
-        <v>2907</v>
+        <v>2927</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>2417</v>
       </c>
-      <c r="C39" s="26" t="s">
-        <v>2904</v>
-      </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
+      <c r="C39" s="33" t="s">
+        <v>2924</v>
+      </c>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="27" t="s">
-        <v>2908</v>
+      <c r="A40" s="34" t="s">
+        <v>2928</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="17" t="s">
-        <v>2910</v>
+        <v>2930</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="17" t="s">
-        <v>2911</v>
+        <v>2931</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="17" t="s">
-        <v>2912</v>
+        <v>2932</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" s="17" t="s">
-        <v>2913</v>
+        <v>2933</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>2909</v>
+        <v>2929</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="17" t="s">
-        <v>2914</v>
+        <v>2934</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="28">
+      <c r="A46" s="35">
         <v>300</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="28" t="s">
-        <v>2916</v>
+      <c r="A47" s="35" t="s">
+        <v>2936</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="28" t="s">
-        <v>2917</v>
+      <c r="A48" s="35" t="s">
+        <v>2937</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>2915</v>
+        <v>2935</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="17" t="s">
-        <v>2918</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>2919</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>2919</v>
+        <v>2938</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>2939</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>2939</v>
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
     </row>
     <row r="50" ht="14.25">
       <c r="A50" s="17" t="s">
-        <v>2920</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>2919</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>2919</v>
+        <v>2940</v>
+      </c>
+      <c r="B50" s="33" t="s">
+        <v>2939</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>2939</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="17" t="s">
-        <v>2921</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>2919</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>2919</v>
+        <v>2941</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>2939</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>2939</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="17" t="s">
-        <v>2922</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>2919</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>2919</v>
+        <v>2942</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>2939</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>2939</v>
       </c>
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
     </row>
     <row r="53" ht="14.25">
       <c r="A53" s="17" t="s">
-        <v>2923</v>
+        <v>2943</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>2924</v>
+        <v>2944</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>2924</v>
+        <v>2944</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
     </row>
     <row r="54" ht="14.25">
       <c r="A54" s="17" t="s">
-        <v>2925</v>
+        <v>2945</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>2926</v>
+        <v>2946</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>2926</v>
+        <v>2946</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
@@ -37312,7 +37541,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2927</v>
+        <v>2947</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>3</v>
@@ -37329,15 +37558,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2928</v>
+        <v>2948</v>
       </c>
       <c r="B2" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2930</v>
+        <v>2950</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>2419</v>
@@ -37345,15 +37574,15 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2931</v>
+        <v>2951</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2932</v>
+        <v>2952</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>2290</v>
@@ -37361,15 +37590,15 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2933</v>
+        <v>2953</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>2934</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2935</v>
+        <v>2955</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>2419</v>
@@ -37377,7 +37606,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2936</v>
+        <v>2956</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>2404</v>
@@ -37385,7 +37614,7 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>2937</v>
+        <v>2957</v>
       </c>
       <c r="B9" t="s">
         <v>2404</v>
@@ -37393,31 +37622,31 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>2938</v>
+        <v>2958</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>2939</v>
+        <v>2959</v>
       </c>
       <c r="B11" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>2940</v>
+        <v>2960</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>2934</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>2941</v>
+        <v>2961</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>2419</v>
@@ -37425,47 +37654,47 @@
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>2942</v>
+        <v>2962</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>2943</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>2944</v>
+        <v>2964</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>2945</v>
+        <v>2965</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>2939</v>
+        <v>2959</v>
       </c>
       <c r="B17" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>2946</v>
+        <v>2966</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>2947</v>
+        <v>2967</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>2419</v>
@@ -37473,7 +37702,7 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>2948</v>
+        <v>2968</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>2419</v>
@@ -37481,7 +37710,7 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>2949</v>
+        <v>2969</v>
       </c>
       <c r="B21" t="s">
         <v>2419</v>
@@ -37489,7 +37718,7 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>2950</v>
+        <v>2970</v>
       </c>
       <c r="B22" t="s">
         <v>2334</v>
@@ -37497,7 +37726,7 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>2951</v>
+        <v>2971</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>2334</v>
@@ -37505,18 +37734,18 @@
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>2952</v>
+        <v>2972</v>
       </c>
       <c r="B24" t="s">
-        <v>2934</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
-        <v>2953</v>
+        <v>2973</v>
       </c>
       <c r="B25" t="s">
-        <v>2929</v>
+        <v>2949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>